<commit_message>
feat [05/03]: update gat_top_wrapper.v, fixing SPMM.sv
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\capstone_project_important\exports_1_3_11_46\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VLSI\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726E566F-9FF8-49D9-B087-E7845DEBD25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF0A8D7-F3A8-4380-899C-80D7993E8FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="13980" windowHeight="11304" xr2:uid="{55869166-5A30-41E5-9330-ED053189522E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18700" xr2:uid="{55869166-5A30-41E5-9330-ED053189522E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -152,7 +152,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +184,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -270,11 +270,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +299,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -306,16 +324,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,134 +691,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AB8BA2-0636-4FE5-800E-DBF73F09E7F2}">
-  <dimension ref="C6:J28"/>
+  <dimension ref="C6:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="46.69921875" customWidth="1"/>
-    <col min="5" max="5" width="16.09765625" customWidth="1"/>
-    <col min="6" max="7" width="14.3984375" customWidth="1"/>
-    <col min="8" max="9" width="13.8984375" customWidth="1"/>
-    <col min="10" max="10" width="13.3984375" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="46.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+    <col min="7" max="10" width="14.36328125" customWidth="1"/>
+    <col min="11" max="13" width="13.90625" customWidth="1"/>
+    <col min="14" max="14" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:10">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="5" t="s">
+    <row r="6" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="16"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="3:10">
-      <c r="C7" s="7" t="s">
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="J7" s="3"/>
+      <c r="K7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="L7" s="3"/>
+      <c r="M7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="3:10">
-      <c r="C8" s="7" t="s">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="3:10">
-      <c r="C9" s="7" t="s">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="14">
         <v>13264</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="12">
+      <c r="F9" s="17"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="14">
         <v>12383</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="3:10">
-      <c r="C10" s="7"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C10" s="10"/>
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="14">
         <v>169</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="12">
+      <c r="F10" s="17"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="14">
         <v>100</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="3:10">
-      <c r="C11" s="7"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C11" s="10"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="14">
         <v>242101</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="3">
+      <c r="F11" s="17"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="3">
         <v>399089</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="3:10">
-      <c r="C12" s="7" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C12" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -786,40 +852,56 @@
       <c r="E12" s="3">
         <v>628</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="20">
+        <v>11</v>
+      </c>
+      <c r="G12" s="3">
         <v>27995</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="20">
+        <v>16</v>
+      </c>
+      <c r="I12" s="3">
         <v>502</v>
       </c>
-      <c r="H12" s="3">
+      <c r="J12" s="20">
+        <v>10</v>
+      </c>
+      <c r="K12" s="3">
         <v>33785</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="3:10">
-      <c r="C13" s="7"/>
+      <c r="L12" s="23">
+        <v>15</v>
+      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C13" s="10"/>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="3">
         <v>-475</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="21"/>
+      <c r="G13" s="3">
         <v>-23626</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="21"/>
+      <c r="I13" s="3">
         <v>-443</v>
       </c>
-      <c r="H13" s="3">
+      <c r="J13" s="21"/>
+      <c r="K13" s="3">
         <v>-11874</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="3:10">
-      <c r="C14" s="8" t="s">
+      <c r="L13" s="24"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C14" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -828,140 +910,184 @@
       <c r="E14" s="3">
         <v>153215</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="20">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3">
         <v>2927847</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="20">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3">
         <v>304107</v>
       </c>
-      <c r="H14" s="3">
+      <c r="J14" s="20">
+        <v>20</v>
+      </c>
+      <c r="K14" s="3">
         <v>3373443</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="C15" s="9"/>
+      <c r="L14" s="20">
+        <v>23</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C15" s="12"/>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="3">
         <v>-133798</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="22"/>
+      <c r="G15" s="3">
         <v>-5110004</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="22"/>
+      <c r="I15" s="3">
         <v>-27743</v>
       </c>
-      <c r="H15" s="3">
+      <c r="J15" s="22"/>
+      <c r="K15" s="3">
         <v>-1065822</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="9"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C16" s="12"/>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="3">
         <v>219831</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="22"/>
+      <c r="G16" s="3">
         <v>3526502</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="22"/>
+      <c r="I16" s="3">
         <v>359391</v>
       </c>
-      <c r="H16" s="3">
+      <c r="J16" s="22"/>
+      <c r="K16" s="3">
         <v>3446933</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" s="9"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C17" s="12"/>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
-      <c r="F17" s="3">
-        <v>0</v>
-      </c>
+      <c r="F17" s="21"/>
       <c r="G17" s="3">
         <v>0</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="21"/>
+      <c r="I17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="3:10">
-      <c r="C18" s="9"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="21"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C18" s="12"/>
       <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="3">
         <v>107</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18" s="20">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3">
         <v>107</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="20">
+        <v>8</v>
+      </c>
+      <c r="I18" s="3">
         <v>87</v>
       </c>
-      <c r="H18" s="3">
+      <c r="J18" s="20">
+        <v>8</v>
+      </c>
+      <c r="K18" s="3">
         <v>105</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="3:10">
-      <c r="C19" s="9"/>
+      <c r="L18" s="20">
+        <v>8</v>
+      </c>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C19" s="12"/>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
-      <c r="F19" s="3">
-        <v>0</v>
-      </c>
+      <c r="F19" s="21"/>
       <c r="G19" s="3">
         <v>0</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="21"/>
+      <c r="I19" s="3">
         <v>0</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="3:10">
-      <c r="C20" s="10"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="21"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="3">
         <v>11</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
         <v>15</v>
       </c>
-      <c r="G20" s="3">
+      <c r="H20" s="3"/>
+      <c r="I20" s="3">
         <v>12</v>
       </c>
-      <c r="H20" s="3">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3">
         <v>15</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="3:10">
-      <c r="C21" s="8" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C21" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -970,120 +1096,144 @@
       <c r="E21" s="4">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="G21" s="4">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4">
         <v>1.54742504910672E+26</v>
       </c>
-      <c r="H21" s="4">
+      <c r="J21" s="4"/>
+      <c r="K21" s="4">
         <v>4.05648192073033E+31</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="3:10">
-      <c r="C22" s="9"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C22" s="12"/>
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3">
         <v>1</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="3"/>
+      <c r="I22" s="3">
         <v>1</v>
       </c>
-      <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="3:10">
-      <c r="C23" s="9"/>
+      <c r="K22" s="3">
+        <v>1</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="4">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="4"/>
+      <c r="G23" s="4">
         <v>1.6242798234512301E+32</v>
       </c>
-      <c r="G23" s="4">
+      <c r="H23" s="4"/>
+      <c r="I23" s="4">
         <v>4.3532663185685503E+26</v>
       </c>
-      <c r="H23" s="4">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4">
         <v>4.0584626247931898E+31</v>
       </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="3:10">
-      <c r="C24" s="9"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C24" s="12"/>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E24" s="3">
         <v>2</v>
       </c>
-      <c r="F24" s="3">
-        <v>2</v>
-      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3">
         <v>2</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3">
         <v>2</v>
       </c>
-      <c r="I24" s="3"/>
       <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="3:10">
-      <c r="C25" s="9"/>
+      <c r="K24" s="3">
+        <v>2</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C25" s="12"/>
       <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3">
         <v>1</v>
       </c>
-      <c r="G25" s="3">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3">
         <v>0.99902439024390199</v>
       </c>
-      <c r="H25" s="3">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3">
         <v>1</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="3:10">
-      <c r="C26" s="10"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C26" s="13"/>
       <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="4">
         <v>1.32348898008484E-23</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="4"/>
+      <c r="G26" s="4">
         <v>3.2311711862532501E-27</v>
       </c>
-      <c r="G26" s="4">
+      <c r="H26" s="4"/>
+      <c r="I26" s="4">
         <v>4.2068066130999898E-5</v>
       </c>
-      <c r="H26" s="4">
+      <c r="J26" s="4"/>
+      <c r="K26" s="4">
         <v>2.5243548967072299E-29</v>
       </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="3:10">
-      <c r="C27" s="7" t="s">
+      <c r="L26" s="4"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C27" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
@@ -1092,43 +1242,64 @@
       <c r="E27" s="3">
         <v>627.99999999897</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3">
         <v>27778.6</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3"/>
+      <c r="I27" s="3">
         <v>447.593170731707</v>
       </c>
-      <c r="H27" s="3">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3">
         <v>33784.252867952098</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="3:10">
-      <c r="C28" s="7"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C28" s="10"/>
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="F28" s="3">
-        <v>0</v>
-      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="3">
         <v>0</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="3"/>
+      <c r="I28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="3"/>
       <c r="J28" s="3"/>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
+  <mergeCells count="28">
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C9:C11"/>
@@ -1137,10 +1308,10 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C14:C20"/>
     <mergeCell ref="C21:C26"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix [12/03]: fix wrapper
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VLSI\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF0A8D7-F3A8-4380-899C-80D7993E8FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC32CF57-234A-493A-A9F0-3C181749D01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18700" xr2:uid="{55869166-5A30-41E5-9330-ED053189522E}"/>
   </bookViews>
@@ -170,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,7 +179,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,66 +302,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -693,14 +738,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0AB8BA2-0636-4FE5-800E-DBF73F09E7F2}">
   <dimension ref="C6:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="12.36328125" customWidth="1"/>
-    <col min="4" max="4" width="46.7265625" customWidth="1"/>
+    <col min="4" max="4" width="41.81640625" customWidth="1"/>
     <col min="5" max="5" width="16.08984375" customWidth="1"/>
     <col min="6" max="6" width="13.90625" customWidth="1"/>
     <col min="7" max="10" width="14.36328125" customWidth="1"/>
@@ -709,594 +754,581 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="8" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="8" t="s">
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="9"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="J7" s="28"/>
+      <c r="K7" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="28"/>
       <c r="M7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="14"/>
+      <c r="I8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="29"/>
+      <c r="K8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="29"/>
       <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="15">
         <v>13264</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="14">
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="30">
         <v>12383</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="6"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C10" s="10"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="15">
         <v>169</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="14">
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="30">
         <v>100</v>
       </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="6"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C11" s="10"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="15">
         <v>242101</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="3">
+      <c r="F11" s="16"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="28">
         <v>399089</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="14">
         <v>628</v>
       </c>
       <c r="F12" s="20">
         <v>11</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="14">
         <v>27995</v>
       </c>
       <c r="H12" s="20">
         <v>16</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="28">
         <v>502</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="34">
         <v>10</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="28">
         <v>33785</v>
       </c>
-      <c r="L12" s="23">
-        <v>15</v>
+      <c r="L12" s="34">
+        <v>16</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C13" s="10"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="14">
         <v>-475</v>
       </c>
       <c r="F13" s="21"/>
-      <c r="G13" s="3">
+      <c r="G13" s="14">
         <v>-23626</v>
       </c>
       <c r="H13" s="21"/>
-      <c r="I13" s="3">
+      <c r="I13" s="28">
         <v>-443</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="3">
+      <c r="J13" s="35"/>
+      <c r="K13" s="28">
         <v>-11874</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="35"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="14">
         <v>153215</v>
       </c>
       <c r="F14" s="20">
         <v>19</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="14">
         <v>2927847</v>
       </c>
       <c r="H14" s="20">
         <v>24</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="28">
         <v>304107</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="34">
         <v>20</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="28">
         <v>3373443</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="34">
         <v>23</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C15" s="12"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="14">
         <v>-133798</v>
       </c>
       <c r="F15" s="22"/>
-      <c r="G15" s="3">
+      <c r="G15" s="14">
         <v>-5110004</v>
       </c>
       <c r="H15" s="22"/>
-      <c r="I15" s="3">
+      <c r="I15" s="28">
         <v>-27743</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="3">
+      <c r="J15" s="36"/>
+      <c r="K15" s="28">
         <v>-1065822</v>
       </c>
-      <c r="L15" s="22"/>
+      <c r="L15" s="36"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C16" s="12"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="14">
         <v>219831</v>
       </c>
       <c r="F16" s="22"/>
-      <c r="G16" s="3">
+      <c r="G16" s="14">
         <v>3526502</v>
       </c>
       <c r="H16" s="22"/>
-      <c r="I16" s="3">
+      <c r="I16" s="28">
         <v>359391</v>
       </c>
-      <c r="J16" s="22"/>
-      <c r="K16" s="3">
+      <c r="J16" s="36"/>
+      <c r="K16" s="28">
         <v>3446933</v>
       </c>
-      <c r="L16" s="22"/>
+      <c r="L16" s="36"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C17" s="12"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="14">
         <v>0</v>
       </c>
       <c r="F17" s="21"/>
-      <c r="G17" s="3">
+      <c r="G17" s="14">
         <v>0</v>
       </c>
       <c r="H17" s="21"/>
-      <c r="I17" s="3">
+      <c r="I17" s="28">
         <v>0</v>
       </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="3">
+      <c r="J17" s="35"/>
+      <c r="K17" s="28">
         <v>0</v>
       </c>
-      <c r="L17" s="21"/>
+      <c r="L17" s="35"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C18" s="12"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="14">
         <v>107</v>
       </c>
       <c r="F18" s="20">
         <v>8</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="14">
         <v>107</v>
       </c>
       <c r="H18" s="20">
         <v>8</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="28">
         <v>87</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="34">
         <v>8</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="28">
         <v>105</v>
       </c>
-      <c r="L18" s="20">
+      <c r="L18" s="34">
         <v>8</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C19" s="12"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="14">
         <v>0</v>
       </c>
       <c r="F19" s="21"/>
-      <c r="G19" s="3">
+      <c r="G19" s="14">
         <v>0</v>
       </c>
       <c r="H19" s="21"/>
-      <c r="I19" s="3">
+      <c r="I19" s="28">
         <v>0</v>
       </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="3">
+      <c r="J19" s="35"/>
+      <c r="K19" s="28">
         <v>0</v>
       </c>
-      <c r="L19" s="21"/>
+      <c r="L19" s="35"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C20" s="13"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="14">
         <v>11</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3">
+      <c r="F20" s="14"/>
+      <c r="G20" s="14">
         <v>15</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3">
+      <c r="H20" s="14"/>
+      <c r="I20" s="28">
         <v>12</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3">
+      <c r="J20" s="28"/>
+      <c r="K20" s="28">
         <v>15</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="28"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="23">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4">
+      <c r="F21" s="23"/>
+      <c r="G21" s="23">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4">
+      <c r="H21" s="23"/>
+      <c r="I21" s="37">
         <v>1.54742504910672E+26</v>
       </c>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4">
+      <c r="J21" s="37"/>
+      <c r="K21" s="37">
         <v>4.05648192073033E+31</v>
       </c>
-      <c r="L21" s="4"/>
+      <c r="L21" s="37"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C22" s="12"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="14">
         <v>1</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3">
+      <c r="F22" s="14"/>
+      <c r="G22" s="14">
         <v>1</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3">
+      <c r="H22" s="14"/>
+      <c r="I22" s="28">
         <v>1</v>
       </c>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3">
+      <c r="J22" s="28"/>
+      <c r="K22" s="28">
         <v>1</v>
       </c>
-      <c r="L22" s="3"/>
+      <c r="L22" s="28"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C23" s="12"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="23">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4">
+      <c r="F23" s="23"/>
+      <c r="G23" s="23">
         <v>1.6242798234512301E+32</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4">
+      <c r="H23" s="23"/>
+      <c r="I23" s="37">
         <v>4.3532663185685503E+26</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4">
+      <c r="J23" s="37"/>
+      <c r="K23" s="37">
         <v>4.0584626247931898E+31</v>
       </c>
-      <c r="L23" s="4"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C24" s="12"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="14">
         <v>2</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3">
+      <c r="F24" s="14"/>
+      <c r="G24" s="14">
         <v>2</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3">
+      <c r="H24" s="14"/>
+      <c r="I24" s="28">
         <v>2</v>
       </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3">
+      <c r="J24" s="28"/>
+      <c r="K24" s="28">
         <v>2</v>
       </c>
-      <c r="L24" s="3"/>
+      <c r="L24" s="28"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C25" s="12"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="14">
         <v>1</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3">
+      <c r="F25" s="14"/>
+      <c r="G25" s="14">
         <v>1</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3">
+      <c r="H25" s="14"/>
+      <c r="I25" s="28">
         <v>0.99902439024390199</v>
       </c>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3">
+      <c r="J25" s="28"/>
+      <c r="K25" s="28">
         <v>1</v>
       </c>
-      <c r="L25" s="3"/>
+      <c r="L25" s="28"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C26" s="13"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="23">
         <v>1.32348898008484E-23</v>
       </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4">
+      <c r="F26" s="23"/>
+      <c r="G26" s="23">
         <v>3.2311711862532501E-27</v>
       </c>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4">
+      <c r="H26" s="23"/>
+      <c r="I26" s="37">
         <v>4.2068066130999898E-5</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4">
+      <c r="J26" s="37"/>
+      <c r="K26" s="37">
         <v>2.5243548967072299E-29</v>
       </c>
-      <c r="L26" s="4"/>
+      <c r="L26" s="37"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="14">
         <v>627.99999999897</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3">
+      <c r="F27" s="14"/>
+      <c r="G27" s="14">
         <v>27778.6</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3">
+      <c r="H27" s="14"/>
+      <c r="I27" s="28">
         <v>447.593170731707</v>
       </c>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3">
+      <c r="J27" s="28"/>
+      <c r="K27" s="28">
         <v>33784.252867952098</v>
       </c>
-      <c r="L27" s="3"/>
+      <c r="L27" s="28"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C28" s="10"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="14">
         <v>0</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3">
+      <c r="F28" s="14"/>
+      <c r="G28" s="14">
         <v>0</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3">
+      <c r="H28" s="14"/>
+      <c r="I28" s="28">
         <v>0</v>
       </c>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3">
+      <c r="J28" s="28"/>
+      <c r="K28" s="28">
         <v>0</v>
       </c>
-      <c r="L28" s="3"/>
+      <c r="L28" s="28"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="J18:J19"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="M6:N6"/>
@@ -1312,6 +1344,19 @@
     <mergeCell ref="I10:K10"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat [22/03]: optimize logic to increase F
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VLSI\Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC32CF57-234A-493A-A9F0-3C181749D01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53139AC-547D-456A-A9CA-70F47AC0A706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="30940" windowHeight="18700" xr2:uid="{55869166-5A30-41E5-9330-ED053189522E}"/>
   </bookViews>
@@ -302,71 +302,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -378,6 +324,48 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,7 +375,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -399,7 +393,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -739,7 +739,7 @@
   <dimension ref="C6:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="H16" sqref="H16:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,581 +754,596 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="24" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="4" t="s">
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="5"/>
+      <c r="N6" s="21"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="28" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28" t="s">
+      <c r="J7" s="10"/>
+      <c r="K7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="29" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29" t="s">
+      <c r="J8" s="11"/>
+      <c r="K8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="29"/>
+      <c r="L8" s="11"/>
       <c r="M8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="29">
         <v>13264</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="30">
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="26">
         <v>12383</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="33"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C10" s="6"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="29">
         <v>169</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="30">
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="26">
         <v>100</v>
       </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="33"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C11" s="6"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="29">
         <v>242101</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="28">
+      <c r="F11" s="30"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="10">
         <v>399089</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="22" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="5">
         <v>628</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="35">
         <v>11</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="5">
         <v>27995</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="35">
         <v>16</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="10">
         <v>502</v>
       </c>
-      <c r="J12" s="34">
+      <c r="J12" s="32">
         <v>10</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="10">
         <v>33785</v>
       </c>
-      <c r="L12" s="34">
+      <c r="L12" s="32">
         <v>16</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C13" s="6"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="5">
         <v>-475</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="14">
+      <c r="F13" s="37"/>
+      <c r="G13" s="5">
         <v>-23626</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="28">
+      <c r="H13" s="37"/>
+      <c r="I13" s="10">
         <v>-443</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="28">
+      <c r="J13" s="33"/>
+      <c r="K13" s="10">
         <v>-11874</v>
       </c>
-      <c r="L13" s="35"/>
+      <c r="L13" s="33"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="5">
         <v>153215</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="35">
         <v>19</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="5">
         <v>2927847</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="35">
         <v>24</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="10">
         <v>304107</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="32">
         <v>20</v>
       </c>
-      <c r="K14" s="28">
+      <c r="K14" s="10">
         <v>3373443</v>
       </c>
-      <c r="L14" s="34">
+      <c r="L14" s="32">
         <v>23</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C15" s="8"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="5">
         <v>-133798</v>
       </c>
-      <c r="F15" s="22"/>
-      <c r="G15" s="14">
+      <c r="F15" s="36"/>
+      <c r="G15" s="5">
         <v>-5110004</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="28">
+      <c r="H15" s="36"/>
+      <c r="I15" s="10">
         <v>-27743</v>
       </c>
-      <c r="J15" s="36"/>
-      <c r="K15" s="28">
+      <c r="J15" s="34"/>
+      <c r="K15" s="10">
         <v>-1065822</v>
       </c>
-      <c r="L15" s="36"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C16" s="8"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="5">
         <v>219831</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="14">
+      <c r="F16" s="36"/>
+      <c r="G16" s="5">
         <v>3526502</v>
       </c>
-      <c r="H16" s="22"/>
-      <c r="I16" s="28">
+      <c r="H16" s="36">
+        <v>23</v>
+      </c>
+      <c r="I16" s="10">
         <v>359391</v>
       </c>
-      <c r="J16" s="36"/>
-      <c r="K16" s="28">
+      <c r="J16" s="34"/>
+      <c r="K16" s="10">
         <v>3446933</v>
       </c>
-      <c r="L16" s="36"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C17" s="8"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="5">
         <v>0</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="14">
+      <c r="F17" s="37"/>
+      <c r="G17" s="5">
         <v>0</v>
       </c>
-      <c r="H17" s="21"/>
-      <c r="I17" s="28">
+      <c r="H17" s="37"/>
+      <c r="I17" s="10">
         <v>0</v>
       </c>
-      <c r="J17" s="35"/>
-      <c r="K17" s="28">
+      <c r="J17" s="33"/>
+      <c r="K17" s="10">
         <v>0</v>
       </c>
-      <c r="L17" s="35"/>
+      <c r="L17" s="33"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C18" s="8"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="5">
         <v>107</v>
       </c>
-      <c r="F18" s="20">
+      <c r="F18" s="35">
         <v>8</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="5">
         <v>107</v>
       </c>
-      <c r="H18" s="20">
+      <c r="H18" s="35">
         <v>8</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="10">
         <v>87</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="32">
         <v>8</v>
       </c>
-      <c r="K18" s="28">
+      <c r="K18" s="10">
         <v>105</v>
       </c>
-      <c r="L18" s="34">
+      <c r="L18" s="32">
         <v>8</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C19" s="8"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="5">
         <v>0</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="14">
+      <c r="F19" s="37"/>
+      <c r="G19" s="5">
         <v>0</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="28">
+      <c r="H19" s="37"/>
+      <c r="I19" s="10">
         <v>0</v>
       </c>
-      <c r="J19" s="35"/>
-      <c r="K19" s="28">
+      <c r="J19" s="33"/>
+      <c r="K19" s="10">
         <v>0</v>
       </c>
-      <c r="L19" s="35"/>
+      <c r="L19" s="33"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C20" s="9"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="5">
         <v>11</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14">
+      <c r="F20" s="5"/>
+      <c r="G20" s="5">
         <v>15</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="28">
+      <c r="H20" s="5"/>
+      <c r="I20" s="10">
         <v>12</v>
       </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10">
         <v>15</v>
       </c>
-      <c r="L20" s="28"/>
+      <c r="L20" s="10"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="23" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="8">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23">
+      <c r="F21" s="8"/>
+      <c r="G21" s="8">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="37">
+      <c r="H21" s="8"/>
+      <c r="I21" s="13">
         <v>1.54742504910672E+26</v>
       </c>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37">
+      <c r="J21" s="13"/>
+      <c r="K21" s="13">
         <v>4.05648192073033E+31</v>
       </c>
-      <c r="L21" s="37"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C22" s="8"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="5">
         <v>1</v>
       </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5">
         <v>1</v>
       </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="28">
+      <c r="H22" s="5"/>
+      <c r="I22" s="10">
         <v>1</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10">
         <v>1</v>
       </c>
-      <c r="L22" s="28"/>
+      <c r="L22" s="10"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C23" s="8"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="8">
         <v>1.62259276829213E+32</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23">
+      <c r="F23" s="8"/>
+      <c r="G23" s="8">
         <v>1.6242798234512301E+32</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="37">
+      <c r="H23" s="8"/>
+      <c r="I23" s="13">
         <v>4.3532663185685503E+26</v>
       </c>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37">
+      <c r="J23" s="13"/>
+      <c r="K23" s="13">
         <v>4.0584626247931898E+31</v>
       </c>
-      <c r="L23" s="37"/>
+      <c r="L23" s="13"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C24" s="8"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="5">
         <v>2</v>
       </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14">
+      <c r="F24" s="5"/>
+      <c r="G24" s="5">
         <v>2</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="28">
+      <c r="H24" s="5"/>
+      <c r="I24" s="10">
         <v>2</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28">
+      <c r="J24" s="10"/>
+      <c r="K24" s="10">
         <v>2</v>
       </c>
-      <c r="L24" s="28"/>
+      <c r="L24" s="10"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C25" s="8"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="5">
         <v>1</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14">
+      <c r="F25" s="5"/>
+      <c r="G25" s="5">
         <v>1</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="28">
+      <c r="H25" s="5"/>
+      <c r="I25" s="10">
         <v>0.99902439024390199</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28">
+      <c r="J25" s="10"/>
+      <c r="K25" s="10">
         <v>1</v>
       </c>
-      <c r="L25" s="28"/>
+      <c r="L25" s="10"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C26" s="9"/>
+      <c r="C26" s="25"/>
       <c r="D26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="8">
         <v>1.32348898008484E-23</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23">
+      <c r="F26" s="8"/>
+      <c r="G26" s="8">
         <v>3.2311711862532501E-27</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="37">
+      <c r="H26" s="8"/>
+      <c r="I26" s="13">
         <v>4.2068066130999898E-5</v>
       </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37">
+      <c r="J26" s="13"/>
+      <c r="K26" s="13">
         <v>2.5243548967072299E-29</v>
       </c>
-      <c r="L26" s="37"/>
+      <c r="L26" s="13"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="22" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="5">
         <v>627.99999999897</v>
       </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14">
+      <c r="F27" s="5"/>
+      <c r="G27" s="5">
         <v>27778.6</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="28">
+      <c r="H27" s="5"/>
+      <c r="I27" s="10">
         <v>447.593170731707</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28">
+      <c r="J27" s="10"/>
+      <c r="K27" s="10">
         <v>33784.252867952098</v>
       </c>
-      <c r="L27" s="28"/>
+      <c r="L27" s="10"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.35">
-      <c r="C28" s="6"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="5">
         <v>0</v>
       </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5">
         <v>0</v>
       </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="28">
+      <c r="H28" s="5"/>
+      <c r="I28" s="10">
         <v>0</v>
       </c>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28">
+      <c r="J28" s="10"/>
+      <c r="K28" s="10">
         <v>0</v>
       </c>
-      <c r="L28" s="28"/>
+      <c r="L28" s="10"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="M6:N6"/>
@@ -1345,18 +1360,6 @@
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L14:L17"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J17"/>
-    <mergeCell ref="J18:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>